<commit_message>
[30-10-2023][Rey] Final Progress Pre Paper
</commit_message>
<xml_diff>
--- a/script/13-10-2023_AlgoEdge.xlsx
+++ b/script/13-10-2023_AlgoEdge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="5">
   <si>
     <t>Algorithm</t>
   </si>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,7 +419,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>192</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -452,7 +452,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>128</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -540,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -551,171 +551,149 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>11</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18">
-        <v>420</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>266</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20">
-        <v>273</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21">
-        <v>192</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>128</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>108</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24">
-        <v>277</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="C25">
-        <v>272</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26">
-        <v>203</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27">
-        <v>222</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30">
         <v>116</v>
       </c>
     </row>

</xml_diff>